<commit_message>
main.py -> Calling extract_sql_from_xml() repeatedly on multiple files
sql_extractor.py ->
Add source_file column to result JSON/Excel
</commit_message>
<xml_diff>
--- a/output/sql_result.xlsx
+++ b/output/sql_result.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,25 +430,30 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>FILE</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>SQL_ID</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>SQL_TYPE</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>주석</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>AS-IS 쿼리</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>TO-BE 쿼리</t>
         </is>
@@ -457,25 +462,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>sample\sampleSQL.xml</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>getUserList</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>select</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>사용자 목록 조회</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>SELECT user_id, user_name FROM TBL_USER WHERE user_status = 'Y'</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>SELECT id, name FROM USERS WHERE user_status = 'Y'</t>
         </is>
@@ -484,25 +494,30 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>sample\sampleSQL.xml</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>getOrderList</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>select</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>주문 목록 조회</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>SELECT order_id, user_id, amount FROM TBL_ORDER WHERE amount &gt; 1000</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>SELECT id, id, total_amt FROM ORDERS WHERE total_amt &gt; 1000</t>
         </is>

</xml_diff>

<commit_message>
refactoring main.py -> add compare result converted
</commit_message>
<xml_diff>
--- a/output/sql_result.xlsx
+++ b/output/sql_result.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,7 +467,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>getUserList</t>
+          <t>retrieveLnRatList</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -477,49 +477,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>사용자 목록 조회</t>
+          <t>융자요율관리 조회(BLOBI070)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SELECT user_id, user_name FROM TBL_USER WHERE user_status = 'Y'</t>
+          <t>SELECT /* SQL_ID : Qblo001m_01DAO.retrieveLnRatList */ LN_GDS_CD AS lnGdsCd /* 융자상품코드 */ , LN_GDS_NM AS lnGdsNm /* 융자상품명 */ , CRDT_EVLT_GRD_CD AS crdtEvltGrdCd /* 신용평가등급코드 */ , CRDT_EVLT_GRD_NM AS crdtEvltGrdNm /* 신용평가등급명 */ , LN_RAT_SEQ AS lnRatSeq /* 융자요율일련번호 */ , LN_RAT_DCD AS lnRatDcd /* 융자요율구분 */ , LN_RAT_DCD_NM AS lnRatDcdNm /* 융자요율구분명 */ , LN_MGNF AS lnMgnf /* 융자배율 */ , LN_INRT AS lnInrt /* 융자이율 */ , LN_RAT_STRT_DT AS lnRatStrtDt /* 융자요율시작일자 */ , LN_RAT_END_DT AS lnRatEndDt /* 융자요율종료일자 */ , US_YN AS usYn /* 사용여부 */ , RMRK AS rmrk /* 비고 */ FROM ( SELECT A.LN_GDS_CD , (SELECT GDS_NM FROM BCO001M B WHERE A.LN_GDS_CD = B.GDS_CD AND BSNS_CLSF_CD = '3001') AS LN_GDS_NM , A.CRDT_EVLT_GRD_CD , SF_SCO_CDNM('CRDT_EVLT_GRD_CD', A.CRDT_EVLT_GRD_CD) AS CRDT_EVLT_GRD_NM , A.LN_RAT_SEQ , A.LN_RAT_DCD , SF_SCO_CDNM('LN_RAT_DCD', A.LN_RAT_DCD) AS LN_RAT_DCD_NM , DECODE(SUBSTR(TO_CHAR(A.LN_MGNF),0,1),'.','0'||TO_CHAR(A.LN_MGNF),A.LN_MGNF) AS LN_MGNF , DECODE(SUBSTR(TO_CHAR(A.LN_INRT),0,1),'.','0'||TO_CHAR(A.LN_INRT),A.LN_INRT) AS LN_INRT , A.LN_RAT_STRT_DT , A.LN_RAT_END_DT , A.US_YN , A.RMRK FROM BLO001M A WHERE (trim(#lnGdsCd#) IS NULL OR A.LN_GDS_CD = #lnGdsCd#) AND (trim(#crdtEvltGrdCd#) IS NULL OR A.CRDT_EVLT_GRD_CD = #crdtEvltGrdCd#) AND ((trim(#lnRatDcd#) IS NULL AND A.LN_RAT_DCD IN ('0007','0008','0009')) OR A.LN_RAT_DCD = #lnRatDcd#) AND A.LN_MGNF LIKE '%'||#lnMgnf#||'%' AND A.LN_INRT LIKE '%'||#lnInrt#||'%' AND (trim(#lnRatStrtDt#) IS NULL OR A.LN_RAT_STRT_DT = #lnRatStrtDt#) AND (trim(#usYn#) IS NULL OR A.US_YN = #usYn#) AND (trim(#rmrk#) IS NULL OR A.RMRK LIKE '%'||#rmrk#||'%') AND A.LN_GDS_CD &gt;= NVL(#nextKey1#, ' ') AND ((A.LN_GDS_CD &gt; #nextKey1#) OR (A.LN_GDS_CD = #nextKey1# AND A.CRDT_EVLT_GRD_CD &gt; #nextKey2#) OR (A.LN_GDS_CD = #nextKey1# AND A.CRDT_EVLT_GRD_CD = #nextKey2# AND A.LN_RAT_SEQ &gt;= #nextKey3#) ) ORDER BY A.LN_GDS_CD, A.CRDT_EVLT_GRD_CD, A.LN_RAT_SEQ ) WHERE ROWNUM &lt;= #rowCount# + 1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>SELECT id, name FROM USERS WHERE user_status = 'Y'</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>sample\sampleSQL.xml</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>getOrderList</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>주문 목록 조회</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>SELECT order_id, user_id, amount FROM TBL_ORDER WHERE amount &gt; 1000</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>SELECT id, id, total_amt FROM ORDERS WHERE total_amt &gt; 1000</t>
+          <t>SELECT /* SQL_ID : Qblo001m_01DAO.retrieveLnRatList */ PRODUCT_CD AS lnGdsCd /* 융자상품코드 */ , LN_GDS_NM AS lnGdsNm /* 융자상품명 */ , CREDIT_CD AS crdtEvltGrdCd /* 신용평가등급코드 */ , CRDT_EVLT_GRD_NM AS crdtEvltGrdNm /* 신용평가등급명 */ , RATE_SEQ AS lnRatSeq /* 융자요율일련번호 */ , RATE_TYPE AS lnRatDcd /* 융자요율구분 */ , LN_RAT_DCD_NM AS lnRatDcdNm /* 융자요율구분명 */ , MAGNIFICATION AS lnMgnf /* 융자배율 */ , INTEREST_RATE AS lnInrt /* 융자이율 */ , START_DATE AS lnRatStrtDt /* 융자요율시작일자 */ , END_DATE AS lnRatEndDt /* 융자요율종료일자 */ , USE_YN AS usYn /* 사용여부 */ , REMARK AS rmrk /* 비고 */ FROM ( SELECT A.PRODUCT_CD , (SELECT PRODUCT_NAME FROM PRODUCT B WHERE A.PRODUCT_CD = B.GDS_CD AND BSNS_CLSF_CD = '3001') AS LN_GDS_NM , A.CREDIT_CD , SF_SCO_CDNM('CREDIT_CD', A.CREDIT_CD) AS CRDT_EVLT_GRD_NM , A.RATE_SEQ , A.RATE_TYPE , SF_SCO_CDNM('RATE_TYPE', A.RATE_TYPE) AS LN_RAT_DCD_NM , DECODE(SUBSTR(TO_CHAR(A.MAGNIFICATION),0,1),'.','0'||TO_CHAR(A.MAGNIFICATION),A.MAGNIFICATION) AS MAGNIFICATION , DECODE(SUBSTR(TO_CHAR(A.INTEREST_RATE),0,1),'.','0'||TO_CHAR(A.INTEREST_RATE),A.INTEREST_RATE) AS INTEREST_RATE , A.START_DATE , A.END_DATE , A.USE_YN , A.REMARK FROM LN_RATE A WHERE (trim(#lnGdsCd#) IS NULL OR A.PRODUCT_CD = #lnGdsCd#) AND (trim(#crdtEvltGrdCd#) IS NULL OR A.CREDIT_CD = #crdtEvltGrdCd#) AND ((trim(#lnRatDcd#) IS NULL AND A.RATE_TYPE IN ('0007','0008','0009')) OR A.RATE_TYPE = #lnRatDcd#) AND A.MAGNIFICATION LIKE '%'||#lnMgnf#||'%' AND A.INTEREST_RATE LIKE '%'||#lnInrt#||'%' AND (trim(#lnRatStrtDt#) IS NULL OR A.START_DATE = #lnRatStrtDt#) AND (trim(#usYn#) IS NULL OR A.USE_YN = #usYn#) AND (trim(#rmrk#) IS NULL OR A.REMARK LIKE '%'||#rmrk#||'%') AND A.PRODUCT_CD &gt;= NVL(#nextKey1#, ' ') AND ((A.PRODUCT_CD &gt; #nextKey1#) OR (A.PRODUCT_CD = #nextKey1# AND A.CREDIT_CD &gt; #nextKey2#) OR (A.PRODUCT_CD = #nextKey1# AND A.CREDIT_CD = #nextKey2# AND A.RATE_SEQ &gt;= #nextKey3#) ) ORDER BY A.PRODUCT_CD, A.CREDIT_CD, A.RATE_SEQ ) WHERE ROWNUM &lt;= #rowCount# + 1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
complete  "case when" test -> next : case when + join, join, union... etc
</commit_message>
<xml_diff>
--- a/output/sql_result.xlsx
+++ b/output/sql_result.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>retrieveLnRatList</t>
+          <t>retrieveCmsUnmbCrdtInrtRt</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -477,17 +477,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>융자요율관리 조회(BLOBI070)</t>
+          <t>CMS 자동이체 처리 위한 이자율, 3개월이하 연체이자율, 3개월초과 연체이자율 조회</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SELECT /* SQL_ID : Qblo001m_01DAO.retrieveLnRatList */ LN_GDS_CD AS lnGdsCd /* 융자상품코드 */ , LN_GDS_NM AS lnGdsNm /* 융자상품명 */ , CRDT_EVLT_GRD_CD AS crdtEvltGrdCd /* 신용평가등급코드 */ , CRDT_EVLT_GRD_NM AS crdtEvltGrdNm /* 신용평가등급명 */ , LN_RAT_SEQ AS lnRatSeq /* 융자요율일련번호 */ , LN_RAT_DCD AS lnRatDcd /* 융자요율구분 */ , LN_RAT_DCD_NM AS lnRatDcdNm /* 융자요율구분명 */ , LN_MGNF AS lnMgnf /* 융자배율 */ , LN_INRT AS lnInrt /* 융자이율 */ , LN_RAT_STRT_DT AS lnRatStrtDt /* 융자요율시작일자 */ , LN_RAT_END_DT AS lnRatEndDt /* 융자요율종료일자 */ , US_YN AS usYn /* 사용여부 */ , RMRK AS rmrk /* 비고 */ FROM ( SELECT A.LN_GDS_CD , (SELECT GDS_NM FROM BCO001M B WHERE A.LN_GDS_CD = B.GDS_CD AND BSNS_CLSF_CD = '3001') AS LN_GDS_NM , A.CRDT_EVLT_GRD_CD , SF_SCO_CDNM('CRDT_EVLT_GRD_CD', A.CRDT_EVLT_GRD_CD) AS CRDT_EVLT_GRD_NM , A.LN_RAT_SEQ , A.LN_RAT_DCD , SF_SCO_CDNM('LN_RAT_DCD', A.LN_RAT_DCD) AS LN_RAT_DCD_NM , DECODE(SUBSTR(TO_CHAR(A.LN_MGNF),0,1),'.','0'||TO_CHAR(A.LN_MGNF),A.LN_MGNF) AS LN_MGNF , DECODE(SUBSTR(TO_CHAR(A.LN_INRT),0,1),'.','0'||TO_CHAR(A.LN_INRT),A.LN_INRT) AS LN_INRT , A.LN_RAT_STRT_DT , A.LN_RAT_END_DT , A.US_YN , A.RMRK FROM BLO001M A WHERE (trim(#lnGdsCd#) IS NULL OR A.LN_GDS_CD = #lnGdsCd#) AND (trim(#crdtEvltGrdCd#) IS NULL OR A.CRDT_EVLT_GRD_CD = #crdtEvltGrdCd#) AND ((trim(#lnRatDcd#) IS NULL AND A.LN_RAT_DCD IN ('0007','0008','0009')) OR A.LN_RAT_DCD = #lnRatDcd#) AND A.LN_MGNF LIKE '%'||#lnMgnf#||'%' AND A.LN_INRT LIKE '%'||#lnInrt#||'%' AND (trim(#lnRatStrtDt#) IS NULL OR A.LN_RAT_STRT_DT = #lnRatStrtDt#) AND (trim(#usYn#) IS NULL OR A.US_YN = #usYn#) AND (trim(#rmrk#) IS NULL OR A.RMRK LIKE '%'||#rmrk#||'%') AND A.LN_GDS_CD &gt;= NVL(#nextKey1#, ' ') AND ((A.LN_GDS_CD &gt; #nextKey1#) OR (A.LN_GDS_CD = #nextKey1# AND A.CRDT_EVLT_GRD_CD &gt; #nextKey2#) OR (A.LN_GDS_CD = #nextKey1# AND A.CRDT_EVLT_GRD_CD = #nextKey2# AND A.LN_RAT_SEQ &gt;= #nextKey3#) ) ORDER BY A.LN_GDS_CD, A.CRDT_EVLT_GRD_CD, A.LN_RAT_SEQ ) WHERE ROWNUM &lt;= #rowCount# + 1</t>
+          <t>SELECT /* SQL_ID : Qblo001m_01DAO.retrieveCmsUnmbCrdtInrtRt */ MAX(lnInrt) AS lnInrt ,MAX(bfrDlyInrt) AS bfrDlyInrt ,MAX(aftrDlyInrt) AS aftrDlyInrt FROM ( SELECT CASE WHEN LN_RAT_DCD = '0007' THEN TO_NUMBER(NVL(SUBSTR(MAX(LN_RAT_STRT_DT || TO_CHAR(LN_INRT)),9), '0')) ELSE 0 END AS lnInrt ,CASE WHEN LN_RAT_DCD = '0008' THEN TO_NUMBER(NVL(SUBSTR(MAX(LN_RAT_STRT_DT || TO_CHAR(LN_INRT)),9), '0')) ELSE 0 END AS bfrDlyInrt ,CASE WHEN LN_RAT_DCD = '0009' THEN TO_NUMBER(NVL(SUBSTR(MAX(LN_RAT_STRT_DT || TO_CHAR(LN_INRT)),9), '0')) ELSE 0 END AS aftrDlyInrt FROM BLO001M A /* BLO_융자요율기본 */ ,( SELECT /*+ index_desc(A PK_BUM206H) */ UNMB_NO ,EVLT_DT ,CRDT_EVLT_GRD_CD FROM BUM206H A /* BUM_조합원등급이력 */ WHERE UNMB_NO = #unmbNo# AND ROWNUM = 1 ) B WHERE 1=1 AND A.LN_GDS_CD = #lnGdsCd# AND A.CRDT_EVLT_GRD_CD = B.CRDT_EVLT_GRD_CD AND A.LN_RAT_DCD IN ('0007','0008','0009') AND A.LN_RAT_STRT_DT &lt;= TO_CHAR(SYSDATE,'YYYYMMDD') AND A.LN_RAT_END_DT &gt;= TO_CHAR(SYSDATE,'YYYYMMDD') AND A.US_YN = 'Y' GROUP BY LN_RAT_DCD )</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>SELECT /* SQL_ID : Qblo001m_01DAO.retrieveLnRatList */ PRODUCT_CD AS lnGdsCd /* 융자상품코드 */ , LN_GDS_NM AS lnGdsNm /* 융자상품명 */ , CREDIT_CD AS crdtEvltGrdCd /* 신용평가등급코드 */ , CRDT_EVLT_GRD_NM AS crdtEvltGrdNm /* 신용평가등급명 */ , RATE_SEQ AS lnRatSeq /* 융자요율일련번호 */ , RATE_TYPE AS lnRatDcd /* 융자요율구분 */ , LN_RAT_DCD_NM AS lnRatDcdNm /* 융자요율구분명 */ , MAGNIFICATION AS lnMgnf /* 융자배율 */ , INTEREST_RATE AS lnInrt /* 융자이율 */ , START_DATE AS lnRatStrtDt /* 융자요율시작일자 */ , END_DATE AS lnRatEndDt /* 융자요율종료일자 */ , USE_YN AS usYn /* 사용여부 */ , REMARK AS rmrk /* 비고 */ FROM ( SELECT A.PRODUCT_CD , (SELECT PRODUCT_NAME FROM PRODUCT B WHERE A.PRODUCT_CD = B.GDS_CD AND BSNS_CLSF_CD = '3001') AS LN_GDS_NM , A.CREDIT_CD , SF_SCO_CDNM('CREDIT_CD', A.CREDIT_CD) AS CRDT_EVLT_GRD_NM , A.RATE_SEQ , A.RATE_TYPE , SF_SCO_CDNM('RATE_TYPE', A.RATE_TYPE) AS LN_RAT_DCD_NM , DECODE(SUBSTR(TO_CHAR(A.MAGNIFICATION),0,1),'.','0'||TO_CHAR(A.MAGNIFICATION),A.MAGNIFICATION) AS MAGNIFICATION , DECODE(SUBSTR(TO_CHAR(A.INTEREST_RATE),0,1),'.','0'||TO_CHAR(A.INTEREST_RATE),A.INTEREST_RATE) AS INTEREST_RATE , A.START_DATE , A.END_DATE , A.USE_YN , A.REMARK FROM LN_RATE A WHERE (trim(#lnGdsCd#) IS NULL OR A.PRODUCT_CD = #lnGdsCd#) AND (trim(#crdtEvltGrdCd#) IS NULL OR A.CREDIT_CD = #crdtEvltGrdCd#) AND ((trim(#lnRatDcd#) IS NULL AND A.RATE_TYPE IN ('0007','0008','0009')) OR A.RATE_TYPE = #lnRatDcd#) AND A.MAGNIFICATION LIKE '%'||#lnMgnf#||'%' AND A.INTEREST_RATE LIKE '%'||#lnInrt#||'%' AND (trim(#lnRatStrtDt#) IS NULL OR A.START_DATE = #lnRatStrtDt#) AND (trim(#usYn#) IS NULL OR A.USE_YN = #usYn#) AND (trim(#rmrk#) IS NULL OR A.REMARK LIKE '%'||#rmrk#||'%') AND A.PRODUCT_CD &gt;= NVL(#nextKey1#, ' ') AND ((A.PRODUCT_CD &gt; #nextKey1#) OR (A.PRODUCT_CD = #nextKey1# AND A.CREDIT_CD &gt; #nextKey2#) OR (A.PRODUCT_CD = #nextKey1# AND A.CREDIT_CD = #nextKey2# AND A.RATE_SEQ &gt;= #nextKey3#) ) ORDER BY A.PRODUCT_CD, A.CREDIT_CD, A.RATE_SEQ ) WHERE ROWNUM &lt;= #rowCount# + 1</t>
+          <t>SELECT /* SQL_ID : Qblo001m_01DAO.retrieveCmsUnmbCrdtInrtRt */ MAX(lnInrt) AS lnInrt ,MAX(bfrDlyInrt) AS bfrDlyInrt ,MAX(aftrDlyInrt) AS aftrDlyInrt FROM ( SELECT CASE WHEN RATE_TYPE = '0007' THEN TO_NUMBER(NVL(SUBSTR(MAX(START_DATE || TO_CHAR(INTEREST_RATE)),9), '0')) ELSE 0 END AS lnInrt ,CASE WHEN RATE_TYPE = '0008' THEN TO_NUMBER(NVL(SUBSTR(MAX(START_DATE || TO_CHAR(INTEREST_RATE)),9), '0')) ELSE 0 END AS bfrDlyInrt ,CASE WHEN RATE_TYPE = '0009' THEN TO_NUMBER(NVL(SUBSTR(MAX(START_DATE || TO_CHAR(INTEREST_RATE)),9), '0')) ELSE 0 END AS aftrDlyInrt FROM LN_RATE A /* BLO_융자요율기본 */ ,( SELECT /*+ index_desc(A PK_BUM206H) */ UNMB_NO ,EVLT_DT ,CREDIT_CD FROM BUM206H A /* BUM_조합원등급이력 */ WHERE UNMB_NO = #unmbNo# AND ROWNUM = 1 ) B WHERE 1=1 AND A.PRODUCT_CD = #lnGdsCd# AND A.CREDIT_CD = B.CREDIT_CD AND A.RATE_TYPE IN ('0007','0008','0009') AND A.START_DATE &lt;= TO_CHAR(SYSDATE,'YYYYMMDD') AND A.END_DATE &gt;= TO_CHAR(SYSDATE,'YYYYMMDD') AND A.USE_YN = 'Y' GROUP BY RATE_TYPE )</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
complete "join" test -> next : union ... etc
</commit_message>
<xml_diff>
--- a/output/sql_result.xlsx
+++ b/output/sql_result.xlsx
@@ -482,12 +482,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SELECT /* SQL_ID : Qblo001m_01DAO.retrieveCmsUnmbCrdtInrtRt */ MAX(lnInrt) AS lnInrt ,MAX(bfrDlyInrt) AS bfrDlyInrt ,MAX(aftrDlyInrt) AS aftrDlyInrt FROM ( SELECT CASE WHEN LN_RAT_DCD = '0007' THEN TO_NUMBER(NVL(SUBSTR(MAX(LN_RAT_STRT_DT || TO_CHAR(LN_INRT)),9), '0')) ELSE 0 END AS lnInrt ,CASE WHEN LN_RAT_DCD = '0008' THEN TO_NUMBER(NVL(SUBSTR(MAX(LN_RAT_STRT_DT || TO_CHAR(LN_INRT)),9), '0')) ELSE 0 END AS bfrDlyInrt ,CASE WHEN LN_RAT_DCD = '0009' THEN TO_NUMBER(NVL(SUBSTR(MAX(LN_RAT_STRT_DT || TO_CHAR(LN_INRT)),9), '0')) ELSE 0 END AS aftrDlyInrt FROM BLO001M A /* BLO_융자요율기본 */ ,( SELECT /*+ index_desc(A PK_BUM206H) */ UNMB_NO ,EVLT_DT ,CRDT_EVLT_GRD_CD FROM BUM206H A /* BUM_조합원등급이력 */ WHERE UNMB_NO = #unmbNo# AND ROWNUM = 1 ) B WHERE 1=1 AND A.LN_GDS_CD = #lnGdsCd# AND A.CRDT_EVLT_GRD_CD = B.CRDT_EVLT_GRD_CD AND A.LN_RAT_DCD IN ('0007','0008','0009') AND A.LN_RAT_STRT_DT &lt;= TO_CHAR(SYSDATE,'YYYYMMDD') AND A.LN_RAT_END_DT &gt;= TO_CHAR(SYSDATE,'YYYYMMDD') AND A.US_YN = 'Y' GROUP BY LN_RAT_DCD )</t>
+          <t>SELECT /* SQL_ID : Qblo100m_01DAO.retrieveLnListPoup */ * FROM ( SELECT a.LN_CNTR_NO as lnCntrNo /* 융자계약번호 */ , SUBSTR(a.LN_CNTR_NO, 1, 16) as lnNo /* 융자번호 */ , SUBSTR(a.LN_CNTR_NO, 19, 2) as lnChnSeq /* 변경회차 */ , a.EXTN_ORD as extnOrd /* 연장차수 */ , substr(a.LN_CNTR_NO, 1, 6)||'-'||substr(a.LN_CNTR_NO, 7, 4)||'-'||substr(a.LN_CNTR_NO, 11, 6)||'('||a.EXTN_ORD||')' as strLnCntrNo /* 융자번호(화면출력) */ , a.LN_GDS_CD as lnGdsCd /* 융자상품코드 */ , (select gds_nm from bco001m b where a.LN_GDS_CD = b.GDS_CD and BSNS_CLSF_CD = '3001') as lnGdsNm /* 융자상품명 */ , a.UNMB_NO as unmbNo /* 조합원 */ , d.ENNM_NM as ennmNm /* 조합원명 */ , a.LN_DT as lnDt /* 융자일자 */ , a.RPYM_FXDT_DT as rpymFxdtDt /* 상환기일일자 */ , a.LN_AMT as lnAmt /* 융자금액 */ , a.JB_BRNC_CD as jbBrncCd /* 업무지점코드 */ , e.PRNT_OFFN as enfcName /* 지점명 */ , a.VLDY_YN as vldyYn /* 유효여부 */ , a.LN_GV_SCD as lnGvScd /* 융자지급상태코드 */ , a.CRDT_GRD_CD as crdtGrdCd , SF_SCO_CDNM('CRDT_GRD_CD', a.CRDT_GRD_CD) as crdtGrdCdNm , a.UNMB_GRD_CD as unmbGrdCd , SF_SCO_CDNM('UNMB_GRD_CD', a.UNMB_GRD_CD) as unmbGrdCdNm , a.UN_INDS_DCD as unIndsDcd , REPLACE(SF_SCO_CDNM('UN_INDS_DCD', a.UN_INDS_DCD), '_', '') as unIndsDcdNm , a.GV_GURN_BLNC as gvGurnBlnc , a.GV_GURN_LMT_AMT as gvGurnLmtAmt FROM BLO100M a /* BLO_융자계약기본 */ , BUM200M c /* BUM_조합원기본 */ , BUM100M d /* BUM_통합고객기본 */ , VI_TM_BRCHXM e /* 사업장_VIEW */ WHERE a.UNMB_NO = c.UNMB_NO AND c.CSTM_NO = d.CSTM_NO(+) AND a.JB_BRNC_CD = e.ENFC_CODE AND a.VLDY_YN = 'Y' AND a.LN_SCD NOT IN ('0010','0011') /* 융자상태코드(상환완료,취소)는 제외 */ AND (#lnCntrNo# IS NULL OR a.LN_CNTR_NO LIKE #lnCntrNo#||'%') AND (#unmbNo# IS NULL OR a.UNMB_NO LIKE #unmbNo#||'%') AND (#unmbNm# IS NULL OR d.ENNM_NM LIKE '%'||#unmbNm#||'%') AND ((#lnGvScd# IS NULL) OR (#lnGvScd# = '4' AND a.LN_GV_SCD = '0004' OR #lnGvScd# &lt;&gt; '4' AND a.LN_GV_SCD &lt;&gt; '0004' )) AND a.UNMB_NO &gt;= NVL(#nextKey1#, ' ') AND ((a.UNMB_NO &gt; #nextKey1# ) OR (a.UNMB_NO = #nextKey1# AND a.LN_CNTR_NO &gt;= #nextKey2#) ) ORDER by a.UNMB_NO, a.LN_CNTR_NO ) WHERE ROWNUM &lt;= #rowCount# + 1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>SELECT /* SQL_ID : Qblo001m_01DAO.retrieveCmsUnmbCrdtInrtRt */ MAX(lnInrt) AS lnInrt ,MAX(bfrDlyInrt) AS bfrDlyInrt ,MAX(aftrDlyInrt) AS aftrDlyInrt FROM ( SELECT CASE WHEN RATE_TYPE = '0007' THEN TO_NUMBER(NVL(SUBSTR(MAX(START_DATE || TO_CHAR(INTEREST_RATE)),9), '0')) ELSE 0 END AS lnInrt ,CASE WHEN RATE_TYPE = '0008' THEN TO_NUMBER(NVL(SUBSTR(MAX(START_DATE || TO_CHAR(INTEREST_RATE)),9), '0')) ELSE 0 END AS bfrDlyInrt ,CASE WHEN RATE_TYPE = '0009' THEN TO_NUMBER(NVL(SUBSTR(MAX(START_DATE || TO_CHAR(INTEREST_RATE)),9), '0')) ELSE 0 END AS aftrDlyInrt FROM LN_RATE A /* BLO_융자요율기본 */ ,( SELECT /*+ index_desc(A PK_BUM206H) */ UNMB_NO ,EVLT_DT ,CREDIT_CD FROM BUM206H A /* BUM_조합원등급이력 */ WHERE UNMB_NO = #unmbNo# AND ROWNUM = 1 ) B WHERE 1=1 AND A.PRODUCT_CD = #lnGdsCd# AND A.CREDIT_CD = B.CREDIT_CD AND A.RATE_TYPE IN ('0007','0008','0009') AND A.START_DATE &lt;= TO_CHAR(SYSDATE,'YYYYMMDD') AND A.END_DATE &gt;= TO_CHAR(SYSDATE,'YYYYMMDD') AND A.USE_YN = 'Y' GROUP BY RATE_TYPE )</t>
+          <t>SELECT /* SQL_ID : Qblo100m_01DAO.retrieveLnListPoup */ * FROM ( SELECT a.CNTR_CD as lnCntrNo /* 융자계약번호 */ , SUBSTR(a.CNTR_CD, 1, 16) as lnNo /* 융자번호 */ , SUBSTR(a.CNTR_CD, 19, 2) as lnChnSeq /* 변경회차 */ , a.EXTN as extnOrd /* 연장차수 */ , substr(a.CNTR_CD, 1, 6)||'-'||substr(a.CNTR_CD, 7, 4)||'-'||substr(a.CNTR_CD, 11, 6)||'('||a.EXTN||')' as strLnCntrNo /* 융자번호(화면출력) */ , a.LN_GDS_CD as lnGdsCd /* 융자상품코드 */ , (select gds_nm from bco001m b where a.LN_GDS_CD = b.GDS_CD and BSNS_CLSF_CD = '3001') as lnGdsNm /* 융자상품명 */ , a.UNMB_NO as unmbNo /* 조합원 */ , d.ENNM_NM as ennmNm /* 조합원명 */ , a.LN_STRT_DT as lnDt /* 융자일자 */ , a.LN_END_DT as rpymFxdtDt /* 상환기일일자 */ , a.LN_AMT as lnAmt /* 융자금액 */ , a.JB_BRNC_CD as jbBrncCd /* 업무지점코드 */ , e.PRNT_OFFN as enfcName /* 지점명 */ , a.VLDY_YN as vldyYn /* 유효여부 */ , a.GV_SCD as lnGvScd /* 융자지급상태코드 */ , a.CRDT_GRD_CD as crdtGrdCd , SF_SCO_CDNM('CRDT_GRD_CD', a.CRDT_GRD_CD) as crdtGrdCdNm , a.UNMB_GRD_CD as unmbGrdCd , SF_SCO_CDNM('UNMB_GRD_CD', a.UNMB_GRD_CD) as unmbGrdCdNm , a.UN_INDS_DCD as unIndsDcd , REPLACE(SF_SCO_CDNM('UN_INDS_DCD', a.UN_INDS_DCD), '_', '') as unIndsDcdNm , a.GV_GURN_BLNC as gvGurnBlnc , a.GV_GURN_LMT_AMT as gvGurnLmtAmt FROM LN_CNTR a /* BLO_융자계약기본 */ , BUM200M c /* BUM_조합원기본 */ , BUM100M d /* BUM_통합고객기본 */ , VI_TM_BRCHXM e /* 사업장_VIEW */ WHERE a.UNMB_NO = c.UNMB_NO AND c.CSTM_NO = d.CSTM_NO(+) AND a.JB_BRNC_CD = e.ENFC_CODE AND a.VLDY_YN = 'Y' AND a.LN_SCD NOT IN ('0010','0011') /* 융자상태코드(상환완료,취소)는 제외 */ AND (#lnCntrNo# IS NULL OR a.CNTR_CD LIKE #lnCntrNo#||'%') AND (#unmbNo# IS NULL OR a.UNMB_NO LIKE #unmbNo#||'%') AND (#unmbNm# IS NULL OR d.ENNM_NM LIKE '%'||#unmbNm#||'%') AND ((#lnGvScd# IS NULL) OR (#lnGvScd# = '4' AND a.GV_SCD = '0004' OR #lnGvScd# &lt;&gt; '4' AND a.GV_SCD &lt;&gt; '0004' )) AND a.UNMB_NO &gt;= NVL(#nextKey1#, ' ') AND ((a.UNMB_NO &gt; #nextKey1# ) OR (a.UNMB_NO = #nextKey1# AND a.CNTR_CD &gt;= #nextKey2#) ) ORDER by a.UNMB_NO, a.CNTR_CD ) WHERE ROWNUM &lt;= #rowCount# + 1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
complete "case when + join" test -> next : union ... etc
</commit_message>
<xml_diff>
--- a/output/sql_result.xlsx
+++ b/output/sql_result.xlsx
@@ -482,12 +482,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SELECT /* SQL_ID : Qblo100m_01DAO.retrieveLnListPoup */ * FROM ( SELECT a.LN_CNTR_NO as lnCntrNo /* 융자계약번호 */ , SUBSTR(a.LN_CNTR_NO, 1, 16) as lnNo /* 융자번호 */ , SUBSTR(a.LN_CNTR_NO, 19, 2) as lnChnSeq /* 변경회차 */ , a.EXTN_ORD as extnOrd /* 연장차수 */ , substr(a.LN_CNTR_NO, 1, 6)||'-'||substr(a.LN_CNTR_NO, 7, 4)||'-'||substr(a.LN_CNTR_NO, 11, 6)||'('||a.EXTN_ORD||')' as strLnCntrNo /* 융자번호(화면출력) */ , a.LN_GDS_CD as lnGdsCd /* 융자상품코드 */ , (select gds_nm from bco001m b where a.LN_GDS_CD = b.GDS_CD and BSNS_CLSF_CD = '3001') as lnGdsNm /* 융자상품명 */ , a.UNMB_NO as unmbNo /* 조합원 */ , d.ENNM_NM as ennmNm /* 조합원명 */ , a.LN_DT as lnDt /* 융자일자 */ , a.RPYM_FXDT_DT as rpymFxdtDt /* 상환기일일자 */ , a.LN_AMT as lnAmt /* 융자금액 */ , a.JB_BRNC_CD as jbBrncCd /* 업무지점코드 */ , e.PRNT_OFFN as enfcName /* 지점명 */ , a.VLDY_YN as vldyYn /* 유효여부 */ , a.LN_GV_SCD as lnGvScd /* 융자지급상태코드 */ , a.CRDT_GRD_CD as crdtGrdCd , SF_SCO_CDNM('CRDT_GRD_CD', a.CRDT_GRD_CD) as crdtGrdCdNm , a.UNMB_GRD_CD as unmbGrdCd , SF_SCO_CDNM('UNMB_GRD_CD', a.UNMB_GRD_CD) as unmbGrdCdNm , a.UN_INDS_DCD as unIndsDcd , REPLACE(SF_SCO_CDNM('UN_INDS_DCD', a.UN_INDS_DCD), '_', '') as unIndsDcdNm , a.GV_GURN_BLNC as gvGurnBlnc , a.GV_GURN_LMT_AMT as gvGurnLmtAmt FROM BLO100M a /* BLO_융자계약기본 */ , BUM200M c /* BUM_조합원기본 */ , BUM100M d /* BUM_통합고객기본 */ , VI_TM_BRCHXM e /* 사업장_VIEW */ WHERE a.UNMB_NO = c.UNMB_NO AND c.CSTM_NO = d.CSTM_NO(+) AND a.JB_BRNC_CD = e.ENFC_CODE AND a.VLDY_YN = 'Y' AND a.LN_SCD NOT IN ('0010','0011') /* 융자상태코드(상환완료,취소)는 제외 */ AND (#lnCntrNo# IS NULL OR a.LN_CNTR_NO LIKE #lnCntrNo#||'%') AND (#unmbNo# IS NULL OR a.UNMB_NO LIKE #unmbNo#||'%') AND (#unmbNm# IS NULL OR d.ENNM_NM LIKE '%'||#unmbNm#||'%') AND ((#lnGvScd# IS NULL) OR (#lnGvScd# = '4' AND a.LN_GV_SCD = '0004' OR #lnGvScd# &lt;&gt; '4' AND a.LN_GV_SCD &lt;&gt; '0004' )) AND a.UNMB_NO &gt;= NVL(#nextKey1#, ' ') AND ((a.UNMB_NO &gt; #nextKey1# ) OR (a.UNMB_NO = #nextKey1# AND a.LN_CNTR_NO &gt;= #nextKey2#) ) ORDER by a.UNMB_NO, a.LN_CNTR_NO ) WHERE ROWNUM &lt;= #rowCount# + 1</t>
+          <t>SELECT A.CUST_ID AS custId, /* 고객 ID */ A.CUST_NM AS custName, /* 고객명 */ B.GRADE_CD AS gradeCode, /* 등급코드 */ SF_SCO_CDNM('GRADE_CD', B.GRADE_CD) AS gradeName, /* 등급명 */ CASE WHEN B.GRADE_CD = 'A' THEN '우수' WHEN B.GRADE_CD = 'B' THEN '일반' ELSE '기타' END AS gradeDesc, /* 등급설명 */ NVL(B.BASE_RATE, 0) AS baseRate, /* 기본요율 */ NVL(B.EXTRA_RATE, 0) AS extraRate, /* 추가요율 */ DECODE(C.REGION_CD, '01', '서울', '02', '부산', '기타') AS regionName, /* 지역명 */ C.REGION_CD AS regionCode, /* 지역코드 */ C.RATE_DESC AS rateDesc /* 요율설명 */ FROM CUSTOMER A LEFT JOIN CUSTOMER_GRADE B ON A.CUST_ID = B.CUST_ID INNER JOIN RATE_INFO C ON B.GRADE_CD = C.GRADE_CD WHERE A.USE_YN = 'Y' AND (TRIM(#custName#) IS NULL OR A.CUST_NM LIKE '%' || #custName# || '%') AND (TRIM(#regionCd#) IS NULL OR C.REGION_CD = #regionCd#) ORDER BY A.CUST_ID</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>SELECT /* SQL_ID : Qblo100m_01DAO.retrieveLnListPoup */ * FROM ( SELECT a.CNTR_CD as lnCntrNo /* 융자계약번호 */ , SUBSTR(a.CNTR_CD, 1, 16) as lnNo /* 융자번호 */ , SUBSTR(a.CNTR_CD, 19, 2) as lnChnSeq /* 변경회차 */ , a.EXTN as extnOrd /* 연장차수 */ , substr(a.CNTR_CD, 1, 6)||'-'||substr(a.CNTR_CD, 7, 4)||'-'||substr(a.CNTR_CD, 11, 6)||'('||a.EXTN||')' as strLnCntrNo /* 융자번호(화면출력) */ , a.LN_GDS_CD as lnGdsCd /* 융자상품코드 */ , (select gds_nm from bco001m b where a.LN_GDS_CD = b.GDS_CD and BSNS_CLSF_CD = '3001') as lnGdsNm /* 융자상품명 */ , a.UNMB_NO as unmbNo /* 조합원 */ , d.ENNM_NM as ennmNm /* 조합원명 */ , a.LN_STRT_DT as lnDt /* 융자일자 */ , a.LN_END_DT as rpymFxdtDt /* 상환기일일자 */ , a.LN_AMT as lnAmt /* 융자금액 */ , a.JB_BRNC_CD as jbBrncCd /* 업무지점코드 */ , e.PRNT_OFFN as enfcName /* 지점명 */ , a.VLDY_YN as vldyYn /* 유효여부 */ , a.GV_SCD as lnGvScd /* 융자지급상태코드 */ , a.CRDT_GRD_CD as crdtGrdCd , SF_SCO_CDNM('CRDT_GRD_CD', a.CRDT_GRD_CD) as crdtGrdCdNm , a.UNMB_GRD_CD as unmbGrdCd , SF_SCO_CDNM('UNMB_GRD_CD', a.UNMB_GRD_CD) as unmbGrdCdNm , a.UN_INDS_DCD as unIndsDcd , REPLACE(SF_SCO_CDNM('UN_INDS_DCD', a.UN_INDS_DCD), '_', '') as unIndsDcdNm , a.GV_GURN_BLNC as gvGurnBlnc , a.GV_GURN_LMT_AMT as gvGurnLmtAmt FROM LN_CNTR a /* BLO_융자계약기본 */ , BUM200M c /* BUM_조합원기본 */ , BUM100M d /* BUM_통합고객기본 */ , VI_TM_BRCHXM e /* 사업장_VIEW */ WHERE a.UNMB_NO = c.UNMB_NO AND c.CSTM_NO = d.CSTM_NO(+) AND a.JB_BRNC_CD = e.ENFC_CODE AND a.VLDY_YN = 'Y' AND a.LN_SCD NOT IN ('0010','0011') /* 융자상태코드(상환완료,취소)는 제외 */ AND (#lnCntrNo# IS NULL OR a.CNTR_CD LIKE #lnCntrNo#||'%') AND (#unmbNo# IS NULL OR a.UNMB_NO LIKE #unmbNo#||'%') AND (#unmbNm# IS NULL OR d.ENNM_NM LIKE '%'||#unmbNm#||'%') AND ((#lnGvScd# IS NULL) OR (#lnGvScd# = '4' AND a.GV_SCD = '0004' OR #lnGvScd# &lt;&gt; '4' AND a.GV_SCD &lt;&gt; '0004' )) AND a.UNMB_NO &gt;= NVL(#nextKey1#, ' ') AND ((a.UNMB_NO &gt; #nextKey1# ) OR (a.UNMB_NO = #nextKey1# AND a.CNTR_CD &gt;= #nextKey2#) ) ORDER by a.UNMB_NO, a.CNTR_CD ) WHERE ROWNUM &lt;= #rowCount# + 1</t>
+          <t>SELECT A.id AS custId, /* 고객 ID */ A.name AS custName, /* 고객명 */ B.grade AS gradeCode, /* 등급코드 */ SF_SCO_CDNM('grade', B.grade) AS gradeName, /* 등급명 */ CASE WHEN B.grade = 'A' THEN '우수' WHEN B.grade = 'B' THEN '일반' ELSE '기타' END AS gradeDesc, /* 등급설명 */ NVL(B.base, 0) AS baseRate, /* 기본요율 */ NVL(B.extra, 0) AS extraRate, /* 추가요율 */ DECODE(C.region, '01', '서울', '02', '부산', '기타') AS regionName, /* 지역명 */ C.region AS regionCode, /* 지역코드 */ C.description AS rateDesc /* 요율설명 */ FROM CUST_TB A LEFT JOIN GRADE_TB B ON A.id = B.id INNER JOIN RATE_TB C ON B.grade = C.grade WHERE A.USE_YN = 'Y' AND (TRIM(#custName#) IS NULL OR A.name LIKE '%' || #custName# || '%') AND (TRIM(#regionCd#) IS NULL OR C.region = #regionCd#) ORDER BY A.id</t>
         </is>
       </c>
     </row>

</xml_diff>